<commit_message>
added 260 sentences to Kisoma Dhopadhola book 2
</commit_message>
<xml_diff>
--- a/Kisoma Dhopadhola.xlsx
+++ b/Kisoma Dhopadhola.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Book2" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="772">
   <si>
     <t>Kitabo Mararyo</t>
   </si>
@@ -1569,6 +1569,768 @@
   </si>
   <si>
     <t xml:space="preserve">  To gik chieni omo ŋwen pere keno aŋwen ma okano i dudi cha</t>
+  </si>
+  <si>
+    <t>Munyo ochulu bende chunye oramo go, to bende chako woth ma kidho limo jatuwo kere</t>
+  </si>
+  <si>
+    <t>Kuchore to mako to chamo go woko kir chwe to chako chwe</t>
+  </si>
+  <si>
+    <t>Onyo kis ogwaŋ kidho neno jatuwo ka owotho kende, kere wacho rigo ni, "Chore gika gime raman swa ma kir ithan kiwinji maber"</t>
+  </si>
+  <si>
+    <t>Munyo kis ogwaŋ chunye ramo go</t>
+  </si>
+  <si>
+    <t>Wach ma tuwo pa kere me to lak kis kamoro</t>
+  </si>
+  <si>
+    <t>Munyo simbwor oti aka paka gochamo ogwange wadi onyo go kinyal ?wech, kinyal nwaŋo girachama, to gonindo piny to chako wacho paka gotuwo swa</t>
+  </si>
+  <si>
+    <t>Chango chango, obedo kere pa ogwange simbwor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Tuwo pa Simbwor</t>
+  </si>
+  <si>
+    <t>Joyiko nyako no to jodok munyo jouro gino</t>
+  </si>
+  <si>
+    <t>To jochako ywak to jouro swa gi ma otimere munyo jonindo</t>
+  </si>
+  <si>
+    <t>Ni jokidho neno to joneno wich nyako no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jome jochiewi de rumachien munyo jowinjo remo ama thon i dak to jopenjere ni, "Aŋo ma thon no?"  </t>
+  </si>
+  <si>
+    <t>To wich mere ketho i dak pi</t>
+  </si>
+  <si>
+    <t>Nyuka odonjo to thumo nyako no</t>
+  </si>
+  <si>
+    <t>Nyako no ni wolwoŋ, ni wokoki jo no jokiwinji</t>
+  </si>
+  <si>
+    <t>Bende apaka otimi, ogwaŋ okelo nindo madwoŋ swa ri wadi nyako no, to donjo i ot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Awachiri wade paran jo jye jowonindi i ot kama ano nindi i iye ni labino oman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To nyako no ywak swa, ka wacho ni, "ŋata ndiri no okedan, ndiri no ochikan ni, i ndelo ma oneni i iye kedi paran</t>
+  </si>
+  <si>
+    <t>Munyo jotieko chiemo to i mako nyako no to i neno kedi pere</t>
+  </si>
+  <si>
+    <t>To nyathi no to neno kedi, to ringo gi ŋwech ka koko ri min ni, "Mama, kedi pa giche nga ber, kendo kichini ma kiwachere kendo ouro swa swa"</t>
+  </si>
+  <si>
+    <t>To munyo por toŋo boke ma malo to nanga ma kore to podho</t>
+  </si>
+  <si>
+    <t>Munyo ringo nyathi mathi be oluwo go"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To min orogo ni, "Ringi aringa ithumi ran boke kwon waŋi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo itedo min guro kwon</t>
+  </si>
+  <si>
+    <t>Munyo kimiti nyutho jo kedi pere</t>
+  </si>
+  <si>
+    <t>Okwero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo otundo pecho openji ni, "Ikedere?"  </t>
+  </si>
+  <si>
+    <t>Nyako oyeyo</t>
+  </si>
+  <si>
+    <t>Ochiko nyako no ni, "Doki, to awacho rin ni kitundo pecho, ongoye nyutho dhano moro jye kedi perin me"</t>
+  </si>
+  <si>
+    <t>Kama okedo go to ketho gagi pensi, ameno ameno to iyi nyako kichin ma kiwachere</t>
+  </si>
+  <si>
+    <t>Nyako obedo piny to okedo go maber swa</t>
+  </si>
+  <si>
+    <t>Kere twodo</t>
+  </si>
+  <si>
+    <t>Ana ogwaŋ ni "Bedi piny, akedin jonicha atieko kedo jo judok"</t>
+  </si>
+  <si>
+    <t>Nyako odwoko go ni, "Aluwo jowotan ma jobino yukome kedi"</t>
+  </si>
+  <si>
+    <t>Munyo otundo pa ogwaŋ, ogwaŋ osangala gi nyako no swa, to penjo go ni, "Aŋo nyako?"</t>
+  </si>
+  <si>
+    <t>Munyo nyako no otieko rego, omako dhoyo to luwo wadi cha i dhoyo pa ogwaŋ ayino</t>
+  </si>
+  <si>
+    <t>Munyo ogwaŋ no oneno boke no, obolo boke no i dhoyo pere</t>
+  </si>
+  <si>
+    <t>Kenyo onwaŋo nitye ogwaŋ ma chamo ji</t>
+  </si>
+  <si>
+    <t>To jowacho rigo dhoyo ma jokidho luwo, to jowacho rigo ni, "Kuma inonwaŋi dhoyo nitye aryo, min onwaŋi wabolo i iye boke, meno ama iluwi"</t>
+  </si>
+  <si>
+    <t>Jonwaŋo go, munyo nyaka chielo kali, aka ripo rego, jokunyalo kuro go</t>
+  </si>
+  <si>
+    <t>To jokidho bothi nyawotigin achiel munwaŋo ongoye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Weyi agik akidhi aomi churo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Rumachien dhako ma oti achiel munyo owok to odoko wacho ni, "O!  Wiyan owili gi churo paran i iy' ogwa?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Adieri ji jowok swa i iye ogwaŋ</t>
+  </si>
+  <si>
+    <t>Jotimo ameno</t>
+  </si>
+  <si>
+    <t>Munyo olach kere bende onwa?o luwo to wacho ama ni, "Kafwodi akitho timi win, ama ŋadi win lwetan mathi me ji ma chango achamo jo, jowowok, aka atho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kani jokidho neno piny obokere pa mach ogwaŋ otundo mager swa min jo opondo yuŋeyi yach nyaka ni wokayi Opiyo, Odongo to chwowi ni wowire ri Odongo, Opiyo to chwowi wire meno dikweth</t>
+  </si>
+  <si>
+    <t>Opiyo gi Odongo Buliri nyuka chango anywoli jo Buliri, fwodi jokuneniye Buliri, biye joneniniye Buliri owero ameno dikweth</t>
+  </si>
+  <si>
+    <t>"Buliro buliri buliriye buliri"</t>
+  </si>
+  <si>
+    <t>Min jo ochako wer kalwoŋo Buliri ama:</t>
+  </si>
+  <si>
+    <t>Nyithindho no jowacho ni, "Lwoŋi ri wan"</t>
+  </si>
+  <si>
+    <t>Winonyali?</t>
+  </si>
+  <si>
+    <t>Min jo to wacho ri nyithindho pere munyo lworo swa ni, "A!  Nyithindho paran, ogwaŋ ago ger swa bino tieko wan kendo obokere ma chulo piny"</t>
+  </si>
+  <si>
+    <t>To jowacho ri min jo ni, "Mama lwoŋi ri wan Buliri, to kubino ibedi yuŋeyi wan"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Munyo joromo i ndelo achiel odikin swa</t>
+  </si>
+  <si>
+    <t>Nyithindho no jochako thedho tonge mabith swa kendo kweth</t>
+  </si>
+  <si>
+    <t>Jowacho ni, "Kale, weyi watemi"</t>
+  </si>
+  <si>
+    <t>Okweri rijo paka ogwaŋ cha ger swa, "Kir an inywolo win apondo aponda"</t>
+  </si>
+  <si>
+    <t>To owacho rijo ni, "Nitye i lul madongo cha"</t>
+  </si>
+  <si>
+    <t>Nyithindho no jopenjo ni, "Ogwaŋ no nitye kune?"</t>
+  </si>
+  <si>
+    <t>Paka ochamo ji otieko kendo, paka ogwaŋ no rach kendo ger swa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Munyo nyithindho no jodongo to oliesa rijo kwoŋ ogwaŋ no ma ilwoŋo ni Buliri</t>
+  </si>
+  <si>
+    <t>Munyo ndelo otundo ma nywol, to nywolo nyithindho aryo rut jo jye yach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Dhako no onwaŋo ni gi iye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ochamo ji otieko i piny no, to kere oweyo dhako acheil kende</t>
+  </si>
+  <si>
+    <t>Chango chango, i piny moro obedo ogwaŋ ma ilwongo ni Buliri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Buliri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Abothi ran weyi akidhi awachi ri wadan ichowo wan konon, inwaŋo ma riek</t>
+  </si>
+  <si>
+    <t>Onyo jatuwo ni tekere wopori kwoŋ ochulu, to ochulu ringo rigo ka wacho ni, "Oido i chamo mamiŋ konon me</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aka odoko jokidwoki ama</t>
+  </si>
+  <si>
+    <t>Ana ochulu ni, "Akinyali choroki bothini, chunyan kutire maber ri neno bathi tiendi wadan ma jobino bothin kenyo"</t>
+  </si>
+  <si>
+    <t>Jatuwo odwoko go ni, "Iŋa kole iluwo kodan gi bor bor chore gika"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wich marapena to wacho ri Kibate ama, "Kibate ikiri inyonan"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wich no jye oluwo gi Kibate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo fwodi ŋwecho kichar ameno to nwaŋo thwol madwoŋ swa manigi wich mere awuchiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kibate obwok swa to Kibate chako achaka ŋwech i dudi kichar</t>
+  </si>
+  <si>
+    <t>Nyuka jye oluwo gi Kibate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Toŋ mecha mere, ni wotoŋ mecha mere, ana mecha ni, ikiri itoŋan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ana gute ni, "Kibate, ikiri itoŋan"</t>
+  </si>
+  <si>
+    <t>Obolo thach piny mako le ni wotoŋ achiel kwoŋ gute me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo omedere to doko nwaŋo gute adek mulile maber swa</t>
+  </si>
+  <si>
+    <t>Kibate obwok swa, to medere gi ŋwech dwaro gute man</t>
+  </si>
+  <si>
+    <t>Ana gute, "Kibate, ikiri itoŋan weyan"</t>
+  </si>
+  <si>
+    <t>Munyo otundo isa, onwaŋo gute mulile swa, obolo thach piny omako le nyaka ni otoŋ gute</t>
+  </si>
+  <si>
+    <t>Kibate oweyo mere pere chimo omako le gi thach kidho toŋo gute</t>
+  </si>
+  <si>
+    <t>Munyo chiemo ana Kibate, "Chimi achima ran ameno ayombere ayombo atoŋ gute achiel, akeli wakethi kenyo"</t>
+  </si>
+  <si>
+    <t>Aneni malo ka orem gute achiel</t>
+  </si>
+  <si>
+    <t>Mere ouro swa Kibate to wacho rigo ni, "Kibate, igeto nedi ot manyien me ma ikiwacho ran abini, akonyini! "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ameno won to mere bino limo go, Kibate osangala swa to rwako mere pere i ot manyien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kibate osangala swa paka mere bino munyo ochowo geto ot pere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kani Kibate kidho neno to limo balwa pa mere pere kawacho rigo paka bino limo go</t>
+  </si>
+  <si>
+    <t>Yiko kageto kunyo, chano, tweyo, bolo, umo gi rwadho, fuyo chwado piny meno jye orumo</t>
+  </si>
+  <si>
+    <t>Ameno won Kibate ochako geto kendo mapiyo swa</t>
+  </si>
+  <si>
+    <t>Ndelo achiel munyo Kibate otieko kidho limo mere, munyo odwoko obedo piny to paro ama, "Bedi achaki geto ot man manyien kamere paran bino won waŋan, anitye i ot manyien"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mere pere bende bino limo Kibate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo onwaŋo jolimere swa, Kibate kidho limo mere pere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kibate me omako mere gi nyawote</t>
+  </si>
+  <si>
+    <t>Chango chango, obedo jal ma ilwoŋo ni Kibate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Kibate</t>
+  </si>
+  <si>
+    <t>Aweyo ran josangala to adwoko ran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Meno min nyithindhi gi rut pere jowinjo siem kendo jotero piny paka piny pajo kendo jomuwok i iye ogwaŋ jofwoyo jo swa madit mere jobedo wade pajo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kunyalo woki kendo otho koro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To ogwaŋ to tho to ŋolo dhakodwoŋ me i iye</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Munyo odonjo kendo i iye ogwaŋ</t>
+  </si>
+  <si>
+    <t>Kogwaŋ no openjo jo ni, "Wachi ran gima itieko neno, jokiluwi meno to jodoŋ adoŋa kenyo"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka i oro jujera omo mach no, jokidwok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kareno yupa kere nitye ogwa manigi mach itunge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To banja loyo Kibate tibolo Kibate i jera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ameno ameno ato wire awira obwol gi kasiki wire awira kir pa kere</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Munyo kendo kidhi pa rwoth man, Kibate oloyo banja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jamilalo loyo banjo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kokidhi pa rwoth man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ameno Kibate oloyo banja jamilalo ojulira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wich dhiaŋ olokere kasiki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Milalo to mako Kibate munyo goyo ndur swa kir pa rwoth tundo pa rwoth marapena riŋo olokere obwol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To obwol ma Kibate otiŋo to lokere riŋo ma chil to kasiki to lokere wich dhiaŋ</t>
+  </si>
+  <si>
+    <t>Munyo fwodi wotho to romo gi jamilalo moro, kere jamilalo no okwali dhiaŋ pere</t>
+  </si>
+  <si>
+    <t>Munyo wacho ni omoki gine mach aoyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To odoko nwaŋo kasiki moro, otiŋo kasiki no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo otundo i dudi koro to nwaŋo obwol otwi ofudho obwol no</t>
+  </si>
+  <si>
+    <t>Kibate oringo, ringo ma kichutho</t>
+  </si>
+  <si>
+    <t>Ti oro go ni, "Kidhi iomi"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nende aneno i dhoyo kacha manago ama yanja swa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nende wi nwaŋan munyo aomo gikipiny, to bedi nende wiwachi ran gima ayaŋo gine</t>
+  </si>
+  <si>
+    <t>An bende, atiyo tich me</t>
+  </si>
+  <si>
+    <t>Odoko penjo jo ni, "Aka bende yanja ri win? "</t>
+  </si>
+  <si>
+    <t>Ana jo ni, "Gi pala"</t>
+  </si>
+  <si>
+    <t>To Kibate penjo jo ni, "Wiy yaŋo g' aŋo?"</t>
+  </si>
+  <si>
+    <t>Kibate otiŋo jatho me kir pecho pajo no tundo, to wachi rigo ni woyaŋi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo jobino to jochako lwoŋo ŋata otho me, kani jokidho neno jomotho me jowok jaryo to jouro swa to jowacho ri Kibate ni wotiŋ jatho</t>
+  </si>
+  <si>
+    <t>Wor munyo otundo jogoli jomotho</t>
+  </si>
+  <si>
+    <t>Kani tundo onwaŋo ni kere joyiko dhano, timako Kibate tiketho ibur, tinwaŋo vata otho me, tiketho malo iwi Kibate, tichako yiko jo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To rwayo ni, "Kono jo ma luwo no jomedho, amadhiye gimoro"</t>
+  </si>
+  <si>
+    <t>Munyo Kibate owinjo wach no jye, to nyaka chore kichar to neno kama nitye i iye pendi kano chiko ithe to winjo luwo korago swa</t>
+  </si>
+  <si>
+    <t>Marawuchiel owacho ni, "Kibate fwodi ni chandirok"</t>
+  </si>
+  <si>
+    <t>Marabich owacho ni, "Weyi win Kibate okadhi"</t>
+  </si>
+  <si>
+    <t>Mara?wen owacho ni, "Kibate weyo uro gi muneno to uro win"</t>
+  </si>
+  <si>
+    <t>Maradek owacho ni, "Kibate lauro win"</t>
+  </si>
+  <si>
+    <t>Mararyo owacho ni, "Kibate nyonin to kunenin"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Go won kende gi dhiaŋ pere bende achiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo jotundo i piny jonwaŋo jachwo no ma ilwoŋo ni Gimoro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ndelo achiel, yach pa Malo jomito bino i piny kiwayaye</t>
+  </si>
+  <si>
+    <t>Gimoro no kareno nitye i piny ka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Obedo bende man ma ilwoŋo ni 'Gimoro'</t>
+  </si>
+  <si>
+    <t>Chango chango, obedo jachwo ma ilwoŋo ni 'Malo' gi Yach gi nyir pere i malo no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Malo gi Gimoro</t>
+  </si>
+  <si>
+    <t>Orumo ameno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo Kilagwech otho otop miyin ato piem gi jarieko itho mikwiya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo kidho tho Ogwal kiwinji rumachien mere to Ogwal oneno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Otemo lwoŋo Ogwal moth moth</t>
+  </si>
+  <si>
+    <t>Munyo wiye wiro go swa to podho i pi to chako nywongo wi pi</t>
+  </si>
+  <si>
+    <t>Kilagwech odoko ameno dwonde aŋwen, marabich</t>
+  </si>
+  <si>
+    <t>Ogwal odwoko go ni, "ŋa?"</t>
+  </si>
+  <si>
+    <t>Ogwal odwoko go malo swa ni, "ŋa?"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo otundo kumogo koro to nyaka wodho dwonde ni pakere wacho ri Ogwal ni "Kururu Ogwal, ayombin, ba!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Firimbi gi kwano orumo Ogwal odonjo i pi to nywongo rigo gi kenyo to Kilagwech ringo pa tho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Jodongo ma jokidho neno ŋwech me jotundo</t>
+  </si>
+  <si>
+    <t>Ameno ndelo otundo ma chako ŋwech</t>
+  </si>
+  <si>
+    <t>Ameno kis Ogwal jye ma pi joniaŋ wach me dwoko ni, "ŋa, ŋa"</t>
+  </si>
+  <si>
+    <t>Kende ni, "ŋa?"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mafwodi sabit no kurumo kere Ogwal odonjo i pi winjirok gi ogwale wadi ni ?ata owinjo ka Kilagwech wacho ni, "Kururu Ogwal, ayombin ba, odwoki wach achiel achiel"</t>
+  </si>
+  <si>
+    <t>Ameno won kole piem ochakere ma ochikere ndelo ma piem ŋwech wobedi iye ato sabit achiel yunyi me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  An aringo i hongo kendo aringo swa, inyalo yomban nedi?</t>
+  </si>
+  <si>
+    <t>Ana Kilagwech ni, "Ogwal weyi ramo chunyan"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Otundo kir munyo kiliesa olokere piem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Paka Ogwal wotho i pi, to Kilagwech wotho i hongo malo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ikiliesa pajo, kis dhano opakere gi nger ma woth pere</t>
+  </si>
+  <si>
+    <t>Chango chango, obedo Kilagwech gi mere pere, Ogwal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Kilagwech gi Ogwal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adongi ran kari olwa pa nera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Onwaŋo anwaŋa mere pere cha fwodi chimo achima malo wi ot kama gute ongoye i iye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kere omiyo go sanduku ma pesa kir gi motoka mukwaŋo go kir pecho pere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo kere oneno go gi mach no, kere osangala swa munyo otito ri kere gima obedo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To tungi ogwaŋ ma dimach to tur, to kwanyo to tero ri kere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Banja ma okelo go pa kere to ogwaŋ to nyiero anyiera swa to podho piny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Paka obwol gi kasiki jolokere rigo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Paka onwaŋo obwol gi kasiki, otiŋo to romo gi mulalo ma okwal dhiaŋ pere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Omiyi go yaŋo jatho cha, rieko muthumo nyuka oori go omo gi yaŋo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Omiyi go tiŋo mulambo no kir pecho pa jome</t>
+  </si>
+  <si>
+    <t>Munyo oyik go gi dhano no, munyo obin golo ŋato yiki no to jowok jaryo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Paka oringo nyuka otundo kama i yiko i iye dhano oŋeyo ni, 'Kono imedho'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Wich no jye kis achiel oluwo gi go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Oweyo mere chimo malo gi paka yen oluwo gi go paka obwok to ringo kichar paka onwa?o thwol ma jawich awuchiel</t>
+  </si>
+  <si>
+    <t>Munyo oori go to munyo otundo both ogwaŋ, ogwaŋ openjo go ni wowachiye rigo gima okelo go i jera, to Kibate chako, paka omako mere, paka ogeto ot, paka mere okidho limo go, gi paka mere owacho rigo paka gute oremi, otiŋo le gi thach kidho toŋo gute</t>
+  </si>
+  <si>
+    <t>Bajo munyo ojok to wacho ri nyare ni, "Meno wach perin, akwerin ni kikadho ikiri gik chien onyo kadhi win gi go ongoye rieko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka nyamin wokadhi, Tho kiyey</t>
+  </si>
+  <si>
+    <t>To ni otem i wondo Tho nedi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To Tho sangala swa kapenjo ni, "Nyaŋono onwaŋo iweyan?"</t>
+  </si>
+  <si>
+    <t>Kani gik, onwaŋo Tho bende otieko dwoko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gwendi bino tho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Nyaŋono gi chwore e jokadho, to i royo bor nyaka to Nyaŋono poyo ni, "O!  Wiyan owili gi kal pa gwendi"</t>
+  </si>
+  <si>
+    <t>Ameno won otieko oro Tho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Iwinjo!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ato ibino nwaŋo Tho odwoko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ka wiyin owil gi gimoro, kipoyo ikiri dwok iom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To ioro Tho bor, tichiko Nyaŋono ni, "Kwanyi kis gimoro perin jye, ikadhi"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kareno Tho kieye bothi Nyaŋono</t>
+  </si>
+  <si>
+    <t>To gosewila Nyaŋano gi kis gimoro gwendi, gi kal ma gwendi lachamo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ato Tho wiye rach, bino chandin</t>
+  </si>
+  <si>
+    <t>Munyo owacho ri bamere, bamere oyeyo go to wacho ri nyare ni, "Kikadho gi Gimoro, Tho wokiri woŋeyi, kendo ikiri ikidhi gi go"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To kareno nitye nyar Malo ilwoŋo ni Nyaŋono omito swa nywomirok gi Gimoro</t>
+  </si>
+  <si>
+    <t>To imiyo go dhok pere jye dok gine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Our to iwacho ni, "Ape!  Kere me gimoro amora adieri!"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ameno won opoy munyo otundo gi wich yen ma tele</t>
+  </si>
+  <si>
+    <t>Sewi pama sanja</t>
+  </si>
+  <si>
+    <t>Kani kidho mako, ape!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo oromo otweyo wich yen pere madwoŋ swa ma tele, to chungo to paro ni, 'Tele ma kitiŋere me, alayeyere nedi?'    </t>
+  </si>
+  <si>
+    <t>Ni kidho baro, to tele bare maber swa, kendo ma boyo swa</t>
+  </si>
+  <si>
+    <t>Weyi atem</t>
+  </si>
+  <si>
+    <t>Tele bende ibaro nedi?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Otundo to wacho ni, "Ha!  An ma gimoro amora me!   </t>
+  </si>
+  <si>
+    <t>Omako le to kadho kir kama di tele</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jye gimoro kokwero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka yen ma go oyo ibaro tele</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ni kidhi ibar rigo yen aoya</t>
+  </si>
+  <si>
+    <t>To odoko jowacho ri Gimoro ni, "Baba ooro wan ni le e e"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo kir bur ochule to jo no jouro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo otieko bolo jye nyaka to lwoŋo jo ni ochowo chiemo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka bende boke to bolo gichien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ochamo manok to chako kwanyo chiemo i boke bolo i bur</t>
+  </si>
+  <si>
+    <t>Kani bolo waŋe to neno bur maluth swa dhu bothe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Anyalo chamo chiemo me jye chowo!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gimoro ologo maber, to bedo piny, to wacho ni, "Ha!  An ma gimoro amora me!"   </t>
+  </si>
+  <si>
+    <t>To ilwoŋo Gimoro chiemo, to iwacho rigo ni, "Eno, wamiyin chiemo no, cham jye"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Yawere tineko dhiaŋ titedo chiemo gi riŋo no jye gipi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo ochowo oketh dhok no gichien</t>
+  </si>
+  <si>
+    <t>Ameno ameno nyuka ochowo dhok pere jye</t>
+  </si>
+  <si>
+    <t>Aka odoko oayi to pie ituŋ dhiaŋ man, to Gimoro wacho ni, "Man kendo eno ma nywol"</t>
+  </si>
+  <si>
+    <t>Ama Gimoro owacho ni, "Ei, dhiaŋ paran eno"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Odoko okel dhok ma chiel man, ama nyaka okondo oayi to pie ituŋ dhia? achiel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gimoro okwero kawacho ni, "Kwoŋ dhok me jye aparan ongoye i iye"</t>
+  </si>
+  <si>
+    <t>Dhok marapena ma okel okondo koayi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Ka doko amedere ameno ma luwo ameno ameno nyuka jorum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Odoko ka no kodere i man, meno amutel nywolo</t>
+  </si>
+  <si>
+    <t>Kareno jotieko chikirok gi okondo ni kinoneni aayi, dhiaŋ ma no pie kwoŋe, meno dhiaŋ Perin</t>
+  </si>
+  <si>
+    <t>Gimoro owacho ni, "Ha!  An ma gimoro amora me! "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo jotundo pa Malo, okel dhok kweth de, tiwacho ri Gimoro ni, "Ere, iwon pa chim dhok perin"</t>
+  </si>
+  <si>
+    <t>Ameno jowotho gi Gimoro kir pa jadwoŋ Malo</t>
+  </si>
+  <si>
+    <t>To Joyeyo ni, "Ei"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Yach no wegi jogik wacho ri Gimoro paka joŋeyo kama dhiaŋ no nitye iye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kareno dhiaŋ no onywol kendo nyithindhe oromo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gimoro ochandere swa kech gi riyo hongo ma lach swa, munyo Gimoro kwiya, ni dhiaŋ pere nitye kune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kareno bajo nigi dhok madit swa i chiel pere</t>
+  </si>
+  <si>
+    <t>Ameno won to joayi kidho kwalo dhiaŋ pa Gimoro to jodwoko gine</t>
+  </si>
+  <si>
+    <t>Ndelo achiel jowacho wegi ni, "Wakidho dwaro dhiaŋ pa Gimoro"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  To Malo uro swa bende</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Tundo pecho joliesaye ri bajo, Malo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo jotieko kiliesa ameno to jodok</t>
+  </si>
+  <si>
+    <t>Jo no jouro swa gima jowinjo no</t>
+  </si>
+  <si>
+    <t>Ana go ni, "Dhiaŋ paran me, ama ka olayo, ama lach mere amadho"</t>
+  </si>
+  <si>
+    <t>Tidok penjo go ni, "To imadh' aŋo?"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Aka ka obolo woyo am' achamo</t>
+  </si>
+  <si>
+    <t>Jalo owacho rijo ni, "An nigi dhiaŋ paran me"</t>
+  </si>
+  <si>
+    <t>Jopenjo go ni, "Inika kendin ichamo aŋo?"</t>
   </si>
 </sst>
 </file>
@@ -2053,9 +2815,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2393,8 +3156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:A447"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4179,10 +4942,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A210"/>
+  <dimension ref="A2:A468"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="C193" sqref="C193"/>
+    <sheetView topLeftCell="A460" workbookViewId="0">
+      <selection activeCell="A484" sqref="A484"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4812,427 +5575,1717 @@
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>9</v>
+        <v>427</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>415</v>
+        <v>461</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>459</v>
+        <v>18</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>18</v>
+        <v>458</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="150" spans="1:1">
-      <c r="A150" t="s">
-        <v>452</v>
+      <c r="A150" s="1" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="152" spans="1:1">
-      <c r="A152" s="1" t="s">
-        <v>450</v>
+      <c r="A152" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>446</v>
+        <v>486</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>462</v>
+        <v>517</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>489</v>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1">
+      <c r="A257" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1">
+      <c r="A259" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1">
+      <c r="A261" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1">
+      <c r="A265" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1">
+      <c r="A267" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1">
+      <c r="A268" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1">
+      <c r="A269" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1">
+      <c r="A270" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1">
+      <c r="A271" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1">
+      <c r="A272" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1">
+      <c r="A273" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1">
+      <c r="A274" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1">
+      <c r="A275" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1">
+      <c r="A276" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1">
+      <c r="A277" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1">
+      <c r="A278" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1">
+      <c r="A279" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1">
+      <c r="A280" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1">
+      <c r="A281" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1">
+      <c r="A282" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1">
+      <c r="A283" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1">
+      <c r="A284" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1">
+      <c r="A285" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1">
+      <c r="A286" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1">
+      <c r="A287" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1">
+      <c r="A288" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1">
+      <c r="A289" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1">
+      <c r="A290" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1">
+      <c r="A291" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1">
+      <c r="A292" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1">
+      <c r="A293" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1">
+      <c r="A294" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1">
+      <c r="A295" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1">
+      <c r="A296" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1">
+      <c r="A297" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1">
+      <c r="A298" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1">
+      <c r="A299" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1">
+      <c r="A300" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1">
+      <c r="A301" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1">
+      <c r="A302" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1">
+      <c r="A303" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1">
+      <c r="A304" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1">
+      <c r="A305" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1">
+      <c r="A306" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1">
+      <c r="A307" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1">
+      <c r="A308" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1">
+      <c r="A309" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1">
+      <c r="A310" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1">
+      <c r="A311" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1">
+      <c r="A312" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1">
+      <c r="A313" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1">
+      <c r="A314" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1">
+      <c r="A315" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1">
+      <c r="A316" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1">
+      <c r="A317" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1">
+      <c r="A318" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1">
+      <c r="A319" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1">
+      <c r="A320" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1">
+      <c r="A321" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1">
+      <c r="A322" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1">
+      <c r="A323" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1">
+      <c r="A324" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1">
+      <c r="A325" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1">
+      <c r="A326" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1">
+      <c r="A327" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1">
+      <c r="A328" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1">
+      <c r="A329" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1">
+      <c r="A330" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1">
+      <c r="A331" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1">
+      <c r="A332" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1">
+      <c r="A333" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1">
+      <c r="A334" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1">
+      <c r="A335" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1">
+      <c r="A336" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1">
+      <c r="A337" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1">
+      <c r="A338" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1">
+      <c r="A339" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1">
+      <c r="A340" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1">
+      <c r="A341" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1">
+      <c r="A342" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1">
+      <c r="A343" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1">
+      <c r="A344" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1">
+      <c r="A345" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1">
+      <c r="A346" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1">
+      <c r="A347" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1">
+      <c r="A348" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1">
+      <c r="A349" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1">
+      <c r="A350" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1">
+      <c r="A351" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1">
+      <c r="A352" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1">
+      <c r="A353" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1">
+      <c r="A354" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1">
+      <c r="A355" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1">
+      <c r="A356" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1">
+      <c r="A357" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1">
+      <c r="A358" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1">
+      <c r="A359" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1">
+      <c r="A360" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1">
+      <c r="A361" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1">
+      <c r="A362" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1">
+      <c r="A363" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1">
+      <c r="A364" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1">
+      <c r="A365" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1">
+      <c r="A366" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1">
+      <c r="A367" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1">
+      <c r="A368" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1">
+      <c r="A369" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1">
+      <c r="A370" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1">
+      <c r="A371" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1">
+      <c r="A372" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1">
+      <c r="A373" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1">
+      <c r="A374" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1">
+      <c r="A375" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1">
+      <c r="A376" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1">
+      <c r="A377" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1">
+      <c r="A378" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1">
+      <c r="A379" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1">
+      <c r="A380" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1">
+      <c r="A381" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1">
+      <c r="A382" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1">
+      <c r="A383" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1">
+      <c r="A384" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1">
+      <c r="A385" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1">
+      <c r="A386" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1">
+      <c r="A387" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1">
+      <c r="A388" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1">
+      <c r="A389" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1">
+      <c r="A390" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1">
+      <c r="A391" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1">
+      <c r="A392" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1">
+      <c r="A393" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1">
+      <c r="A394" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1">
+      <c r="A395" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1">
+      <c r="A396" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1">
+      <c r="A397" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1">
+      <c r="A398" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1">
+      <c r="A399" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1">
+      <c r="A400" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1">
+      <c r="A401" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1">
+      <c r="A402" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1">
+      <c r="A403" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1">
+      <c r="A404" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1">
+      <c r="A405" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1">
+      <c r="A406" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1">
+      <c r="A407" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1">
+      <c r="A408" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1">
+      <c r="A409" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1">
+      <c r="A410" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1">
+      <c r="A411" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1">
+      <c r="A412" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1">
+      <c r="A413" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1">
+      <c r="A414" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1">
+      <c r="A415" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1">
+      <c r="A416" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1">
+      <c r="A417" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1">
+      <c r="A418" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1">
+      <c r="A419" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1">
+      <c r="A420" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1">
+      <c r="A421" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1">
+      <c r="A422" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1">
+      <c r="A423" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1">
+      <c r="A424" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1">
+      <c r="A425" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1">
+      <c r="A426" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1">
+      <c r="A427" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1">
+      <c r="A428" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1">
+      <c r="A429" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1">
+      <c r="A430" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1">
+      <c r="A431" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1">
+      <c r="A432" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1">
+      <c r="A433" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1">
+      <c r="A434" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1">
+      <c r="A435" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1">
+      <c r="A436" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1">
+      <c r="A437" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1">
+      <c r="A438" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1">
+      <c r="A439" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1">
+      <c r="A440" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1">
+      <c r="A441" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1">
+      <c r="A442" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1">
+      <c r="A443" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1">
+      <c r="A444" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1">
+      <c r="A445" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1">
+      <c r="A446" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1">
+      <c r="A447" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1">
+      <c r="A448" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1">
+      <c r="A449" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1">
+      <c r="A450" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1">
+      <c r="A451" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1">
+      <c r="A452" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1">
+      <c r="A453" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1">
+      <c r="A454" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1">
+      <c r="A455" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1">
+      <c r="A456" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1">
+      <c r="A457" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1">
+      <c r="A458" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1">
+      <c r="A459" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1">
+      <c r="A460" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1">
+      <c r="A461" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1">
+      <c r="A462" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1">
+      <c r="A463" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1">
+      <c r="A464" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1">
+      <c r="A465" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1">
+      <c r="A466" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1">
+      <c r="A467" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1">
+      <c r="A468" t="s">
+        <v>702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished combining and gen basic statistics
</commit_message>
<xml_diff>
--- a/Kisoma Dhopadhola.xlsx
+++ b/Kisoma Dhopadhola.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Clean" sheetId="2" r:id="rId1"/>
+    <sheet name="Book 2" sheetId="2" r:id="rId1"/>
+    <sheet name="Book 1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="1124">
   <si>
     <t>Kitabo Mararyo</t>
   </si>
@@ -2552,6 +2553,840 @@
   </si>
   <si>
     <t>Adhola</t>
+  </si>
+  <si>
+    <t>Kitabo Marapena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wafwoyo swa ji jye, somero ma Siwa kod Miganja Praimari. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Okoth Mariko omo kitabo me ma fwonjo Dhopadhola ri nyithindho ma praimari.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medo nyayo kitabo me ri fwonji maber swa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bende inyalo nwaŋo kitabo me .</t>
+  </si>
+  <si>
+    <t>Kitabo me nitye gi kigana kod gikipiny ma fwonji ondiko dwe marabiryo tundo dwe marabuŋwen, 2002.</t>
+  </si>
+  <si>
+    <t>Nyikuta ma Dhopadhola</t>
+  </si>
+  <si>
+    <t>Riwo Nyikuta Aryo</t>
+  </si>
+  <si>
+    <t>Riwo Nyikuta Adek/Aŋwen</t>
+  </si>
+  <si>
+    <t>Agecha gi Dwanyo Wach</t>
+  </si>
+  <si>
+    <t>Jakwakirok jakun</t>
+  </si>
+  <si>
+    <t>Makoko jye wok i tonge</t>
+  </si>
+  <si>
+    <t>ŋata kifwonji wotho gi gimoro yuŋeye</t>
+  </si>
+  <si>
+    <t>Awendo ma lwor ama yindira</t>
+  </si>
+  <si>
+    <t>Jagwondo Jarawanya</t>
+  </si>
+  <si>
+    <t>Jafwoch ama ye?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jakisunga kilogi</t>
+  </si>
+  <si>
+    <t>Theke theke awech jodongo</t>
+  </si>
+  <si>
+    <t>Muwolo loyo muŋwenyere</t>
+  </si>
+  <si>
+    <t>Mwolo pa rombo kimon go dwiro</t>
+  </si>
+  <si>
+    <t>Awendo kingoye gachiero</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ŋaŋo meno thoyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Achiel achiel a wich (kosa kayego)</t>
+  </si>
+  <si>
+    <t>Kuro kwo oloyo ŋaŋo</t>
+  </si>
+  <si>
+    <t>Awendo timo ni che-</t>
+  </si>
+  <si>
+    <t>Chandere aka i nolim</t>
+  </si>
+  <si>
+    <t>Wot gwendi gore i chuŋ machon</t>
+  </si>
+  <si>
+    <t>Kisalaka kiyengere nono</t>
+  </si>
+  <si>
+    <t>Nyakus dhiaŋ kiwoki i kigo nono</t>
+  </si>
+  <si>
+    <t>Ikiri chai bo ma dikado</t>
+  </si>
+  <si>
+    <t>Jambaka nyewo mbiye</t>
+  </si>
+  <si>
+    <t>Jamikwenda wiye bulero</t>
+  </si>
+  <si>
+    <t>Kama olwokere ama kithwo iye</t>
+  </si>
+  <si>
+    <t>Kichami gi rochi</t>
+  </si>
+  <si>
+    <t>Chandi waŋ adhola</t>
+  </si>
+  <si>
+    <t>Kisi ndelo kibedi sabit</t>
+  </si>
+  <si>
+    <t>Koth goyo min gweno loko mbwo?</t>
+  </si>
+  <si>
+    <t>Furi wire</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Koth ma odiechieŋ kigoy ŋata achiel</t>
+  </si>
+  <si>
+    <t>Koth ma ogoyin gi pe</t>
+  </si>
+  <si>
+    <t>Kulo gi bemo</t>
+  </si>
+  <si>
+    <t>Gi 	Athieno Getrude kod Nyafwono Connie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dwanyo Lew</t>
+  </si>
+  <si>
+    <t>Yiwi mamba miti, yiwi mamba miti</t>
+  </si>
+  <si>
+    <t>Amudhe dicha chiemo dho ndelo dho loka dho jwom</t>
+  </si>
+  <si>
+    <t>Waka waka wakawaka ni wakawaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Madhombedhombe patha patha ni patha patha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kwara kidho kudho gwara Gwaragwara</t>
+  </si>
+  <si>
+    <t>Mwodo mwodo mwodere pa mwodo</t>
+  </si>
+  <si>
+    <t>Ochola chor achero machon ma cheŋino Ochieŋ ochiemiye</t>
+  </si>
+  <si>
+    <t>Ochola ocholo Achola chon</t>
+  </si>
+  <si>
+    <t>Okello oleko lek yo loka koro</t>
+  </si>
+  <si>
+    <t>Adhadha odhier g'adher i dhoyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kwany kwer iwey kwinyo</t>
+  </si>
+  <si>
+    <t>Sikoiko</t>
+  </si>
+  <si>
+    <t>Dhiaŋ ka nindo paro aŋo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anitye gi gikipiny adek, kodhi rabwo, diel, gi ondiek. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Atimi nedi aka atiŋ jo jye akal gi jo malawa?  </t>
+  </si>
+  <si>
+    <t>Aka ye paran tiŋo gimoro achiel achiel.</t>
+  </si>
+  <si>
+    <t>Muchungwa ochiek mito afwona.</t>
+  </si>
+  <si>
+    <t>Aŋo ma mwonyo yokin tineno?</t>
+  </si>
+  <si>
+    <t>Opiyo otelo Odongo kimaki.</t>
+  </si>
+  <si>
+    <t>Adhadha langa langa i pendi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antiye gi muchungwa paran i dier malawa.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aka kenyo nitye jajwok.  </t>
+  </si>
+  <si>
+    <t>Atimi nedi aka acham muchungwa?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ageto ot paran ma ongoye dhu ot.  </t>
+  </si>
+  <si>
+    <t>Abedo aŋo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nyathi paran okidho wendo ma ongoye gi nanga to dwoko gine.  </t>
+  </si>
+  <si>
+    <t>Aŋo mofwonjo wan gi ruko kanzo?</t>
+  </si>
+  <si>
+    <t>Gonyi diel iwey loch.</t>
+  </si>
+  <si>
+    <t>Nya pa rwoth okedere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Adhadha otho oweyo kisiwiro.</t>
+  </si>
+  <si>
+    <t>Nyir owaŋo wiy jo.</t>
+  </si>
+  <si>
+    <t>Aŋo mofwonjo wan gi ruko junga?</t>
+  </si>
+  <si>
+    <t>Radwok ma Sikoiko</t>
+  </si>
+  <si>
+    <t>Paro ni kama diel jye nitye gi yer tike aka an a?ata angoye gine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teli tero diel loka, dwoki i omi ondiek bende iteri loka, to idwoko kod diel.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kwany kodhi rabwo bende iteri loka.  </t>
+  </si>
+  <si>
+    <t>Nyaka to i gik omo diel.</t>
+  </si>
+  <si>
+    <t>Nyako othik mito poro</t>
+  </si>
+  <si>
+    <t>Dero</t>
+  </si>
+  <si>
+    <t>Tiendi gal</t>
+  </si>
+  <si>
+    <t>Musalawuyo</t>
+  </si>
+  <si>
+    <t>Kwany tele idwiri gine jajwok aka jajwok wofwoni muchungwa to dwirin gine.</t>
+  </si>
+  <si>
+    <t>Tongweno</t>
+  </si>
+  <si>
+    <t>Maido</t>
+  </si>
+  <si>
+    <t>ŋwen</t>
+  </si>
+  <si>
+    <t>Oseyo</t>
+  </si>
+  <si>
+    <t>Nanasi</t>
+  </si>
+  <si>
+    <t>Alemo oweyo royo</t>
+  </si>
+  <si>
+    <t>Toko</t>
+  </si>
+  <si>
+    <t>Obwol</t>
+  </si>
+  <si>
+    <t>Gimumiyo Gwendi Lworo Otengo</t>
+  </si>
+  <si>
+    <t>Chango chango, gweno jomako mere kod katateŋ.</t>
+  </si>
+  <si>
+    <t>Mere pajo obedo matek swa ma kisi gimoro jye jo kwayere.</t>
+  </si>
+  <si>
+    <t>Ndelo achiel gweno oayi to kidho pa otengo to kwayo go piso ma kwoyo nanga.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo gweno odwoko gi piso to kwoyo gine nanga. </t>
+  </si>
+  <si>
+    <t>Munyo ochowo kwoyo nanga, to kano piso i ot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Otengo okuro ni gweno odwoki ri go piso pere to gweno kudwoko. </t>
+  </si>
+  <si>
+    <t>Ndelo achiel otengo won otiŋere to kidho pa gweno penjo go piso pere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gweno oayi to kidho kama chango no go okano i iye piso to kunwaŋo.</t>
+  </si>
+  <si>
+    <t>Gweno oparo gima go owachi ri jawodhe to ngoye.</t>
+  </si>
+  <si>
+    <t>Rumacheni gweno owacho ri otengo ni "Piso orwenyo ran kama aketho i iye</t>
+  </si>
+  <si>
+    <t>Weyi doko, alatemo rango, ka anwaŋo alakelo rin.</t>
+  </si>
+  <si>
+    <t>Gweno otemo atema yaro piny ni rango ri otengo piso pere to kwero nwaŋo kiri dikin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woki ndelo no kiri konon mere pa gweno kod otengo tu tho atha. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Meno amomiyo ineno gweno yaro piny munyo rango ri otengo piso pere.</t>
+  </si>
+  <si>
+    <t>Aka bende amomiyo otengo chamo nyithindhi gwendi ri piso pere ma gweno orwenyo.</t>
+  </si>
+  <si>
+    <t>Lwaŋino gi Awino</t>
+  </si>
+  <si>
+    <t>Obedo ndelo achiel Awino okidho i sikul, to neno lwaŋino.</t>
+  </si>
+  <si>
+    <t>Lwaŋino oido opie i kor ot ma sikul.</t>
+  </si>
+  <si>
+    <t>To lwaŋino penjo go ni, "Ikidho i kilas perin?"</t>
+  </si>
+  <si>
+    <t>To godwoko, "Eei akidho i kilas."</t>
+  </si>
+  <si>
+    <t>To lwaŋino wacho ni "Kale, abende, akidho i kilas."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lwaŋino omedo luwo ni, "Awino, kidonjo i kilas. "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ikiri nenan; ikiri luwi; ikiri nur.  </t>
+  </si>
+  <si>
+    <t>To neni anena kitabo perin."</t>
+  </si>
+  <si>
+    <t>Munyo gosoma kitabo pere i sikul, to goneno lwaŋino i kor ot.</t>
+  </si>
+  <si>
+    <t>To godiyo nyawote ma bedo gine i kom to wacho ri go ni, "Neni lwaŋino no, goluwo."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To dichiel lwaŋino to pie i waŋe, to nyutho jafwonji pere.  </t>
+  </si>
+  <si>
+    <t>Munyo wacho ni, "Lwaŋino ni waŋan, jafwonji konyan, ikwanyi ran!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jafwonji to konjo pi i kikopo to wacho ni, "Yawi waŋin." </t>
+  </si>
+  <si>
+    <t>To lwoko waŋe to lwaŋino wok i waŋe to ayi to kadho.</t>
+  </si>
+  <si>
+    <t>To ayi to pie i dirisa to bedo iwi dirisa to lwoko waŋe gi tiende.</t>
+  </si>
+  <si>
+    <t>Pusi kod Oyeyo</t>
+  </si>
+  <si>
+    <t>Chango chango, obedo Pusi kod Oyeyo to jomakere mere.</t>
+  </si>
+  <si>
+    <t>Pusi kod Oyeyo jonyewo modhiaŋ pajo to joketho i dak to joŋawo kisalaka.</t>
+  </si>
+  <si>
+    <t>Ndelo achiel Pusi oromo kod Oyeyo to penjo go ni "Ojame, iwok yukune?"</t>
+  </si>
+  <si>
+    <t>Oyeyo owacho rigo ni "Awok kibatisa nyathi paran."</t>
+  </si>
+  <si>
+    <t>Pusi openjo go ni "Ibatisa go ni ŋa?"</t>
+  </si>
+  <si>
+    <t>Oyeyo odwoko ni "Abatisa go ni Onaŋo-de-onaŋo-de-oweyo-i-ganga."</t>
+  </si>
+  <si>
+    <t>Ndelo man doko Pusi oromo kod Oyeyo to penjo go ni "Ojame, iwok yukune?"</t>
+  </si>
+  <si>
+    <t>Oyeyo odwoko ni "Awok kibatisa nyathi paran."</t>
+  </si>
+  <si>
+    <t>Pusi openjo ni "Ibatisa go ni ŋa?"</t>
+  </si>
+  <si>
+    <t>Oyeyo odwoko go ni "Abatisa go ni Onaŋo-de-onaŋo-de-oweyo-i-kore."</t>
+  </si>
+  <si>
+    <t>Oyeyo odwoko go ni "Awok kibatisa nyathi paran."</t>
+  </si>
+  <si>
+    <t>Oyeyo odwoko ni "Abatisa go ni Onaŋo de onaŋo de olwindo."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ndelo achiel Pusi owacho ri Oyeyo ni "Wakidhi walimi mo mawan." </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oyeyo oayi to pondo ri Pusi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pusi won to ayi kidho limo mo kama ndelago jokano iye. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Munyo Pusi otundo onwaŋo anwaŋa dak nono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mo ongoye iye kada nyaka mathin. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pusi odok to kidho rango Oyeyo wacho rigo paka mo ma chango jokano i dak ongoye kada nyaka mathin.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo Oyeyo oneno Pusi obino, Oyeyo oringo to pondo. </t>
+  </si>
+  <si>
+    <t>Pusi owacho ni "Iraŋo Oyeyo onenan to pondo?"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nyutho ni go ama onaŋo mo ma wakano.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wok ndelo no Pusi kuneno Oyeyo to neko aneka to chamo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oyeyo bende koneno Pusi ringo aringa to pondo munyo lworo Pusi.</t>
+  </si>
+  <si>
+    <t>Kwach gi Gweno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chango chango, gwendi gi ogwaŋe jobedo mere swa tek tek. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gwendi gi ogwaŋe jo jye oido jobedo, jochiemo, jonindo i dudi.</t>
+  </si>
+  <si>
+    <t>To dichiel kwach omito tedo ri nyithindhe chiemo to mach ongoye.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To kwach poyo dichiel paka joliesa gi wod gweno kwoŋ gima mako mach.  </t>
+  </si>
+  <si>
+    <t>To munyo kwach okidho to nwaŋo wod gweno ongoye tichiko, godwoko othieno.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo kwach odoko ogik mararyo, kareno chie? liel swa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To kwach dok, kuro kir othieno munyo piny okwe to doko gik. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Maradek to nwaŋo wod gweno munyo nindo.  </t>
+  </si>
+  <si>
+    <t>To temo chiewo go, to wod gweno konyalo chiewi.</t>
+  </si>
+  <si>
+    <t>To kenyo paro bino ri kwach ma kwalo mach.</t>
+  </si>
+  <si>
+    <t>To dimo lum mothwo swa ma nyalo moko piyo piyo.</t>
+  </si>
+  <si>
+    <t>To choko, munyo otieko choko to tiŋo.</t>
+  </si>
+  <si>
+    <t>Okidho kama wod gweno nindo iye.</t>
+  </si>
+  <si>
+    <t>Munyo otundo to ketho lum i wiye wod gweno mach komoko.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mararyo to doko ketho mach doko koliel. </t>
+  </si>
+  <si>
+    <t>Maradek kwach rume to ruda aruda lum i kokoliro wod gweno jye doko mach koliel.</t>
+  </si>
+  <si>
+    <t>To wod gweno chiewi.</t>
+  </si>
+  <si>
+    <t>To neno kwach, obedo chiegin bothi.</t>
+  </si>
+  <si>
+    <t>To wacho ri kwach ni, "Ikiri chore chiegin."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ayawaŋin gi mach ma wiyan.</t>
+  </si>
+  <si>
+    <t>To yengo wiye munyo bwoko kwach paka lawaŋo go.</t>
+  </si>
+  <si>
+    <t>Kwach koringo kosa kodhire gi chien.</t>
+  </si>
+  <si>
+    <t>To kwach wacho ri wod gweno ni, "Gima ni wiyin no, kimach, itwodo."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gi kenyo to kwach lokere ri wod gweno mager. </t>
+  </si>
+  <si>
+    <t>To mito kiri mako wod gweno oneki ri twodo pere.</t>
+  </si>
+  <si>
+    <t>To wod gweno wire gi ŋwech munyo koko ri gwendi wadi jye ni "Kok kok kudee!"(loki Dhopadhola 'Kawagalo kadagala, ilaneko wan!')</t>
+  </si>
+  <si>
+    <t>To joŋwecho gi ŋwech madit swa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wok ndir no gwendi joringo wok i dudi kama oido jobedo iye.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiri gonyo gwendi bedo bothi ji.  </t>
+  </si>
+  <si>
+    <t>Wor jonindo i ot munyo jolworo ogwange.</t>
+  </si>
+  <si>
+    <t>Ochulu gi ŋech</t>
+  </si>
+  <si>
+    <t>Kigana pa Ochulu gi ŋech (gimumiyo ŋech nindo i kero).</t>
+  </si>
+  <si>
+    <t>Chango chango, obedo Ochulu gi ŋech to jomako mere.</t>
+  </si>
+  <si>
+    <t>Ndelo achiel to ŋech wacho ri Ochulu ni okwaŋi go wendo pa ore.</t>
+  </si>
+  <si>
+    <t>Ochulu bende to yeyo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Munyo ndelo otundo to joayi kadho wendo.</t>
+  </si>
+  <si>
+    <t>Munyo jonitye i royo Ochulu ochungo to wacho ri mere pere ni, "Paka wakidho pa or wakiri waor nyingi wan ma kisindelo.</t>
+  </si>
+  <si>
+    <t>Wachwok nyingi wan man ma olwoŋi gine wan."</t>
+  </si>
+  <si>
+    <t>ŋech bende kokwero.</t>
+  </si>
+  <si>
+    <t>Ochulu to wacho ri vech oteli yero nyinge.</t>
+  </si>
+  <si>
+    <t>ŋech to yero nyinge ni 'Jadwong' to Ochulu to yero nyinge ni 'Wendo.'</t>
+  </si>
+  <si>
+    <t>Munyo jotundo pa or ŋech, ti fwoyo gi neno jo swa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Munyo jopecho jowacho ni, "Wafwoyo swa gi neno wendo."</t>
+  </si>
+  <si>
+    <t>Ochulu to wacho ri ŋech, "Ofwoyi gi nenan kendan."</t>
+  </si>
+  <si>
+    <t>To won pecho doko wacho ni, "Keli win ri wendo kom."</t>
+  </si>
+  <si>
+    <t>Ochulu to wacho ni, "Meno jye kom paran."</t>
+  </si>
+  <si>
+    <t>Doko ti wacho ni, "Keli win ri wendo koŋo."</t>
+  </si>
+  <si>
+    <t>Ochulu to wacho ni, "Meno jye koŋo paran." to madho woko jye kende.</t>
+  </si>
+  <si>
+    <t>To i kelo chiemo kareno ŋech kech neko go tek tek swa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To jokidho logo woko, munyo jodwoko chiemo chingi ŋech oido koch paka go patho apatha i lowo. </t>
+  </si>
+  <si>
+    <t>Ochulu to wacho ri go ni "Ojame neni chingin paka koch."</t>
+  </si>
+  <si>
+    <t>Ikiri i kwo ti wiyan pa or, kidhi doko ilogi."</t>
+  </si>
+  <si>
+    <t>To ŋech kidho logo kareno mere pere Ochulu chiemo swa piyo piyo.</t>
+  </si>
+  <si>
+    <t>Munyo ŋech odwoko i dhuweri odoko chinge onwaŋo opoŋiye lowo rupir gowotho gi chinge.</t>
+  </si>
+  <si>
+    <t>Odoko Ochulu wacho ri go ni ogik ologi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Munyo odwoko onwaŋo Ochulu ochowo chamo woko chiemo jye. </t>
+  </si>
+  <si>
+    <t>Ma Odoŋi jye orwako i mugowa(kikapo) pere.</t>
+  </si>
+  <si>
+    <t>Ochulu to lwoŋo, "Wegi pecho omo sendere."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To josewila jo to jodok ma nyawote kochiemo.</t>
+  </si>
+  <si>
+    <t>Munyo jotundo i royo to ŋech gak i dudi ni iye riemo, to ŋwecho yo wiyi Ochulu to lokere simon.</t>
+  </si>
+  <si>
+    <t>Ochulu munyo otundo kama di simon to gweyo munyo wacho ni, "Me ŋech won ama rendere."</t>
+  </si>
+  <si>
+    <t>To ŋech doko ŋwecho aŋwecha malo kama chipa Ochulu ofuro iye to lokere ombokoro.</t>
+  </si>
+  <si>
+    <t>Munyo Ochulu otundo i ndelo to neno ombokoro, okwako dimo to ketho i mugowa pere ka wacho ni,  "Min Awoi me miŋi swa oweyo ombokoyo pa nyathi payan i ndeyo ka."</t>
+  </si>
+  <si>
+    <t>Munyo otundo pecho owacho ri min Awor konjo woko fufa ma nwaŋo otedo.</t>
+  </si>
+  <si>
+    <t>To oro Awor omo mugowa ma nende odwoko gine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Awor otemo tiŋo mugowa to wacho ni mugowa pek swa.</t>
+  </si>
+  <si>
+    <t>To Ochulu wacho ri dhako pere min Awor kidho omo mugowa.</t>
+  </si>
+  <si>
+    <t>Dhako pere bende konyalo tiŋo mugowa.</t>
+  </si>
+  <si>
+    <t>To gowon kidho.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onwaŋo mugowa pek swa, to tiŋo gi meni to wodho i diedipo.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo oyawo mugowa to ŋech woki gi ŋwechi. </t>
+  </si>
+  <si>
+    <t>To Ochulu joriemo swa tek tek to ŋech ŋwecho to yombo jo to donjo i kero.</t>
+  </si>
+  <si>
+    <t>Amomiyo pama ŋech bwoki paro ni Ochulu fwodi riemo go.</t>
+  </si>
+  <si>
+    <t>ŋech ŋwecho to donjo i kero.</t>
+  </si>
+  <si>
+    <t>Merin Adek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chango chango, obedo Wakafundo, Alur, kod Kagujuguju. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jobedo merin matek.</t>
+  </si>
+  <si>
+    <t>Ndelo achiel Wakafundo, Alur kod Kogujuguju joayi to jokidho i katale nyewo dhiaŋ</t>
+  </si>
+  <si>
+    <t>Munyo jotieko nyewo dhiaŋ pajo to joayi dwoko, koth madwoŋ to chako chwe.</t>
+  </si>
+  <si>
+    <t>Merin adek me to jotweyo dhiaŋ pajo i tiendi yath dho thengi ngudo to jokidho bwok koth i pecho machegin.</t>
+  </si>
+  <si>
+    <t>Munyo koth ochok jokidho i tiendi yath ma nende jotweyo iye dhiaŋ pajo jo wo chaki woth pajo to jokunwaŋo dhiaŋ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jodwaro dhiaŋ kisi kamoro jye to jokunwaŋo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jokwo ido jotieko kwalo woko dhiaŋ chon.</t>
+  </si>
+  <si>
+    <t>Wok ndelo no merin adek me jokedho chikirok pajo ama</t>
+  </si>
+  <si>
+    <t>Wakafundo okwoŋere ni doko gokibino neno malo (polo) kama koth owoki iye ma omiyo dhiaŋ pajo okwali.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kir konon me Wakafundo kineni malo.</t>
+  </si>
+  <si>
+    <t>Koneno malo, latho atha.</t>
+  </si>
+  <si>
+    <t>Alur okwoŋere ni doko gokibino piye wi yath ma oido jotweyo iye dhiaŋ pajo aka omiyo jokwo jokwalo.</t>
+  </si>
+  <si>
+    <t>Kagujuguju okwoŋere ni doko gokibino ŋado royo ma jo joluwo munyo jowok i katale.</t>
+  </si>
+  <si>
+    <t>Ka achiel kwoŋ jo otimo gino latho atha gi kenyo.</t>
+  </si>
+  <si>
+    <t>Jadwar</t>
+  </si>
+  <si>
+    <t>Chango chango, obedo jalmoro gi pecho pere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jalo obedo jadwar. </t>
+  </si>
+  <si>
+    <t>Ndelo acheil owacho ri dhako pere gi nyithindho ni jokidhi jodoyi mwogo.</t>
+  </si>
+  <si>
+    <t>Go to kidho dwar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dhako bende oayi gi nyithindho kadho doyo mwogo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I ndelo mwogo no nitye winyo ma chiemo i iye.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dhako no gi nyithindho pere jodoyo mwogo to jochowo woko ndelo.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo winyo me obino chiemo onwaŋo ndelo ler.  </t>
+  </si>
+  <si>
+    <t>Winyo me to chako wer.</t>
+  </si>
+  <si>
+    <t>Dhako me, dhako me</t>
+  </si>
+  <si>
+    <t>Imiyan girachula</t>
+  </si>
+  <si>
+    <t>Abende abino miyin girachula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo gowero ameno to diewo i ndelo to lum doko twi pa gen nende kenyo kufuri.  </t>
+  </si>
+  <si>
+    <t>To gochiemo rigin to yeŋ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo jadwoŋ me odwoko dwar to kidho neno muga ma nende dhako pere gi nyithindho jofuro.  </t>
+  </si>
+  <si>
+    <t>To nwaŋo ndelo oyukino ma ongoye kada lakikwer achiel ma otoŋ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jadwoŋ me odwoko to penjo dhako pere muga.  </t>
+  </si>
+  <si>
+    <t>Dhako owacho rigo ni, "Nende wadoyo adoyo mwogo jye to wachowo."</t>
+  </si>
+  <si>
+    <t>Jadwoŋ me owacho rigo ni, "Ongoye kacha, kada lakikwer ma otoŋ, kada achiel."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yaweremere jadwoŋ me doko odhiro dhako me gi nyithindho kidho doyo mwogo.  </t>
+  </si>
+  <si>
+    <t>Jome jodoyo mwogo doko to jochowo.</t>
+  </si>
+  <si>
+    <t>Munyo winyo me obino to nwaŋo ndelo ler doko to chako wer.</t>
+  </si>
+  <si>
+    <t>Doko to lum twi i ndelo gipi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Munyo jadwoŋ me odwoko dwar to kidho i ndelo neno muga to nwaŋo ni ongoye kama ofuri, kada achiel.  </t>
+  </si>
+  <si>
+    <t>Ka godok penjo dhako to dhako wacho rigo paka jofuro afura ndelo jye.</t>
+  </si>
+  <si>
+    <t>Ndelo maradek jadwoŋ me oayi gi dhako pere gi nyithindho jye to jokidho i ndelo to go bende jye temo furi to weyo munyo dhako gi nyithindho medere gi fur to go kadho dwar</t>
+  </si>
+  <si>
+    <t>Jome jofuro, to jochowo ndelo, to jodoki.</t>
+  </si>
+  <si>
+    <t>Winyo me doko obino to nwaŋo ndelo ler to doko wero ni</t>
+  </si>
+  <si>
+    <t>To dudi twi to gochiemo to yeŋ to kadho.</t>
+  </si>
+  <si>
+    <t>Munyo jadwoŋ me okidho i ndelo onwa?o kir kama go ofuro jye dudi otwi iye.</t>
+  </si>
+  <si>
+    <t>Nitye jawodhe ma onwaŋo go i ndelo to wacho rigo ni, "Nitye gima bino wero i ndelo perin ka otieki furo to dudi twi."</t>
+  </si>
+  <si>
+    <t>Ere dikin ipondi ibino neno.</t>
+  </si>
+  <si>
+    <t>Yaweremere jadwoŋ me doko odhiro dhako gi nyithindho kidho doyo mwogo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> To jadwoŋ me pondo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Munyo dhako gi nyithindho jotieko doy, gowacho ri dhako umo go gi lum aka jodoki.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winyo me doko obino to nwaŋo ndelo ler to chako wer.  </t>
+  </si>
+  <si>
+    <t>Jadwoŋ me ogoyo winyo no, to neko.</t>
   </si>
 </sst>
 </file>
@@ -3384,8 +4219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A846"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A827" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A846"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7626,4 +8461,1412 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:A279"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
+      <selection activeCell="A297" sqref="A297"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="100.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="1" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="1" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="1" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="1" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="1" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="1" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="1" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="1" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="1" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="1" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="1" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="1" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="1" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="1" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="1" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" s="1" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" s="1" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" s="1" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" s="1" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" s="1" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="1" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" s="1" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" s="1" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" s="1" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" s="1" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" s="1" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" s="1" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" s="1" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" s="1" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="1" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" s="1" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" s="1" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" s="1" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" s="1" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1">
+      <c r="A257" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1">
+      <c r="A259" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1">
+      <c r="A261" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1">
+      <c r="A265" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1">
+      <c r="A267" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1">
+      <c r="A268" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1">
+      <c r="A269" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1">
+      <c r="A270" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1">
+      <c r="A271" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1">
+      <c r="A272" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1">
+      <c r="A273" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1">
+      <c r="A274" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1">
+      <c r="A275" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1">
+      <c r="A276" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1">
+      <c r="A277" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1">
+      <c r="A278" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1">
+      <c r="A279" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>